<commit_message>
new folders with milk
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters CATTLE.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters CATTLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/Mac/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CCED44-FA81-7043-BB49-1D8188E8577C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEA1633-79A6-3D44-A8A6-7D8A93E1F853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="28100" windowHeight="16140" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="299">
   <si>
     <t># Initial population</t>
   </si>
@@ -899,9 +899,6 @@
     <t>rpert(10000, 200, 380, 290)</t>
   </si>
   <si>
-    <t>rpert(10000, 8.3, 11.7, 18)</t>
-  </si>
-  <si>
     <t>cattle_trial_CLM_ideal</t>
   </si>
   <si>
@@ -912,12 +909,6 @@
   </si>
   <si>
     <t>cattle_trial_periurban_dairy_ideal</t>
-  </si>
-  <si>
-    <t>rpert(10000, 10, 15, 20)</t>
-  </si>
-  <si>
-    <t>rpert(10000, 250, 380, 290)</t>
   </si>
   <si>
     <t>cattle_trial_CLM_all_mortality_zero</t>
@@ -1073,9 +1064,6 @@
     <t>0.03/12</t>
   </si>
   <si>
-    <t>rpert(75, 540, 330)</t>
-  </si>
-  <si>
     <t>rpert(10000, 0.63, 0.75, 0.69)</t>
   </si>
   <si>
@@ -1206,6 +1194,12 @@
   </si>
   <si>
     <t>rpert(10000, (38324+(0*38324)), (38324+(0*38324)), (38324+(0*38324)))</t>
+  </si>
+  <si>
+    <t>rpert(10000, 75, 540, 330)</t>
+  </si>
+  <si>
+    <t>rpert(10000, 8.3, 18, 11.7)</t>
   </si>
 </sst>
 </file>
@@ -1792,9 +1786,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:AGM159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AV23" sqref="AV23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1863,46 +1857,46 @@
         <v>154</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="31" t="s">
-        <v>199</v>
-      </c>
-      <c r="F1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="L1" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="M1" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="N1" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="P1" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="Q1" s="31" t="s">
         <v>214</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>217</v>
       </c>
       <c r="R1" s="38" t="s">
         <v>155</v>
@@ -1911,43 +1905,43 @@
         <v>156</v>
       </c>
       <c r="T1" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U1" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="V1" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="W1" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="X1" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="V1" s="38" t="s">
+      <c r="Y1" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="W1" s="38" t="s">
+      <c r="Z1" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="X1" s="38" t="s">
+      <c r="AA1" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="AB1" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="Z1" s="38" t="s">
+      <c r="AC1" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="AA1" s="38" t="s">
+      <c r="AD1" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="AB1" s="38" t="s">
+      <c r="AE1" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="AC1" s="38" t="s">
+      <c r="AF1" s="38" t="s">
         <v>226</v>
-      </c>
-      <c r="AD1" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="AE1" s="38" t="s">
-        <v>228</v>
-      </c>
-      <c r="AF1" s="38" t="s">
-        <v>229</v>
       </c>
       <c r="AG1" s="2" t="s">
         <v>195</v>
@@ -1956,43 +1950,43 @@
         <v>196</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AJ1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="AM1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="AV1" s="4"/>
       <c r="AW1" s="4"/>
@@ -2017,7 +2011,7 @@
     </row>
     <row r="2" spans="1:871" s="42" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="43"/>
@@ -9372,7 +9366,7 @@
         <v>162</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F17" s="33" t="s">
         <v>162</v>
@@ -9402,7 +9396,7 @@
         <v>162</v>
       </c>
       <c r="O17" s="55" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="P17" s="33" t="s">
         <v>162</v>
@@ -10336,7 +10330,7 @@
         <v>151</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F18" s="33" t="s">
         <v>151</v>
@@ -10366,7 +10360,7 @@
         <v>151</v>
       </c>
       <c r="O18" s="55" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="P18" s="33" t="s">
         <v>151</v>
@@ -10381,7 +10375,7 @@
         <v>151</v>
       </c>
       <c r="T18" s="48" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="U18" s="17" t="s">
         <v>151</v>
@@ -10411,7 +10405,7 @@
         <v>151</v>
       </c>
       <c r="AD18" s="48" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="AE18" s="17" t="s">
         <v>151</v>
@@ -10426,7 +10420,7 @@
         <v>151</v>
       </c>
       <c r="AI18" s="50" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="AJ18" s="21" t="s">
         <v>151</v>
@@ -10455,8 +10449,8 @@
       <c r="AR18" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="AS18" s="21" t="s">
-        <v>151</v>
+      <c r="AS18" s="50" t="s">
+        <v>270</v>
       </c>
       <c r="AT18" s="21" t="s">
         <v>151</v>
@@ -12293,7 +12287,7 @@
         <v>210</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>256</v>
+        <v>297</v>
       </c>
       <c r="F22" s="33">
         <v>210</v>
@@ -12323,7 +12317,7 @@
         <v>210</v>
       </c>
       <c r="O22" s="55" t="s">
-        <v>256</v>
+        <v>297</v>
       </c>
       <c r="P22" s="33">
         <v>210</v>
@@ -12338,7 +12332,7 @@
         <v>210</v>
       </c>
       <c r="T22" s="48" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="U22" s="17">
         <v>210</v>
@@ -12368,7 +12362,7 @@
         <v>210</v>
       </c>
       <c r="AD22" s="48" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="AE22" s="17">
         <v>210</v>
@@ -12383,7 +12377,7 @@
         <v>197</v>
       </c>
       <c r="AI22" s="50" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="AJ22" s="21" t="s">
         <v>197</v>
@@ -12413,7 +12407,7 @@
         <v>197</v>
       </c>
       <c r="AS22" s="50" t="s">
-        <v>204</v>
+        <v>283</v>
       </c>
       <c r="AT22" s="21" t="s">
         <v>197</v>
@@ -13257,7 +13251,7 @@
         <v>174</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F23" s="33" t="s">
         <v>174</v>
@@ -13287,7 +13281,7 @@
         <v>174</v>
       </c>
       <c r="O23" s="55" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="P23" s="33" t="s">
         <v>174</v>
@@ -13302,7 +13296,7 @@
         <v>1.79</v>
       </c>
       <c r="T23" s="48" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="U23" s="17">
         <v>1.79</v>
@@ -13332,7 +13326,7 @@
         <v>1.79</v>
       </c>
       <c r="AD23" s="48" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="AE23" s="17">
         <v>1.79</v>
@@ -13341,49 +13335,49 @@
         <v>1.79</v>
       </c>
       <c r="AG23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AH23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AI23" s="50" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="AJ23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AK23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AL23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AM23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AN23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AO23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AP23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AQ23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AR23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AS23" s="50" t="s">
-        <v>203</v>
+        <v>284</v>
       </c>
       <c r="AT23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AU23" s="21" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="AV23" s="5"/>
       <c r="AW23" s="5"/>
@@ -18279,49 +18273,49 @@
         <v>0</v>
       </c>
       <c r="AG34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AH34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AI34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AJ34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AK34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AL34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AM34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AN34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AO34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AP34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AQ34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AR34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AS34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AT34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AU34" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AV34" s="5"/>
       <c r="AW34" s="5"/>
@@ -19243,49 +19237,49 @@
         <v>0</v>
       </c>
       <c r="AG35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AH35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AI35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AJ35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AK35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AL35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AM35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AN35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AO35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AP35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AQ35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AR35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AS35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AT35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AU35" s="21" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="AV35" s="5"/>
       <c r="AW35" s="5"/>
@@ -20162,94 +20156,94 @@
         <v>169</v>
       </c>
       <c r="R36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="S36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="T36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="U36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="V36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="W36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="X36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="Y36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="Z36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AA36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AB36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AC36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AD36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AE36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AF36" s="17" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AG36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AH36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AI36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AJ36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AK36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AL36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AM36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AN36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AO36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AP36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AQ36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AR36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AS36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AT36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AU36" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AV36" s="5"/>
       <c r="AW36" s="5"/>
@@ -21126,49 +21120,49 @@
         <v>0</v>
       </c>
       <c r="R37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="S37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="T37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="U37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="V37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="W37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="X37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="Y37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="Z37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AA37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AB37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AC37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AD37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AE37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AF37" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AG37" s="21">
         <v>0</v>
@@ -22093,94 +22087,94 @@
         <v>170</v>
       </c>
       <c r="R38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="S38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="T38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="U38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="V38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="W38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="X38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="Y38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="Z38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="AA38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="AB38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="AC38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="AD38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="AE38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="AF38" s="19" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="AG38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AH38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AI38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AJ38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AK38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AL38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AM38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AN38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AO38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AP38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AQ38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AR38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AS38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AT38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AU38" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AV38" s="5"/>
       <c r="AW38" s="5"/>
@@ -23060,94 +23054,94 @@
         <v>171</v>
       </c>
       <c r="R39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="S39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="T39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="U39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="V39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="W39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="X39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="Y39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="Z39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AA39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AB39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AC39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AD39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AE39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AF39" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AG39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AH39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AI39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AJ39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AK39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AL39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AM39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AN39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AO39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AP39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AQ39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AR39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AS39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AT39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AU39" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AV39" s="5"/>
       <c r="AW39" s="5"/>
@@ -24069,49 +24063,49 @@
         <v>0</v>
       </c>
       <c r="AG40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AH40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AI40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AJ40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AK40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AL40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AM40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AN40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AO40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AP40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AQ40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AR40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AS40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AT40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AU40" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AV40" s="5"/>
       <c r="AW40" s="5"/>
@@ -25059,7 +25053,7 @@
         <v>173</v>
       </c>
       <c r="R43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="S43" s="53">
         <v>0</v>
@@ -25071,16 +25065,16 @@
         <v>0</v>
       </c>
       <c r="V43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="W43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="X43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Y43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Z43" s="53">
         <v>0</v>
@@ -25089,22 +25083,22 @@
         <v>0</v>
       </c>
       <c r="AB43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="AC43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="AD43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="AE43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="AF43" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="AG43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AH43" s="54">
         <v>0</v>
@@ -25116,16 +25110,16 @@
         <v>0</v>
       </c>
       <c r="AK43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AL43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AM43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AN43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AO43" s="54">
         <v>0</v>
@@ -25134,19 +25128,19 @@
         <v>0</v>
       </c>
       <c r="AQ43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AR43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AS43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AT43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AU43" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AV43" s="5"/>
       <c r="AW43" s="5"/>
@@ -26026,7 +26020,7 @@
         <v>172</v>
       </c>
       <c r="R44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="S44" s="53">
         <v>0</v>
@@ -26035,25 +26029,25 @@
         <v>0</v>
       </c>
       <c r="U44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="V44" s="53">
         <v>0</v>
       </c>
       <c r="W44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="X44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="Y44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="Z44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AA44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AB44" s="53">
         <v>0</v>
@@ -26062,13 +26056,13 @@
         <v>0</v>
       </c>
       <c r="AD44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AE44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AF44" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AG44" s="23" t="s">
         <v>181</v>
@@ -27038,7 +27032,7 @@
         <v>171</v>
       </c>
       <c r="AG45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AH45" s="54">
         <v>0</v>
@@ -27047,40 +27041,40 @@
         <v>0</v>
       </c>
       <c r="AJ45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AK45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AL45" s="54">
         <v>0</v>
       </c>
       <c r="AM45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AN45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AO45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AP45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AQ45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AR45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AS45" s="54">
         <v>0</v>
       </c>
       <c r="AT45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AU45" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AV45" s="5"/>
       <c r="AW45" s="5"/>
@@ -27960,7 +27954,7 @@
         <v>181</v>
       </c>
       <c r="R46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="S46" s="53">
         <v>0</v>
@@ -27969,43 +27963,43 @@
         <v>0</v>
       </c>
       <c r="U46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="V46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="W46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="X46" s="53">
         <v>0</v>
       </c>
       <c r="Y46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="Z46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AA46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AB46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AC46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AD46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AE46" s="53">
         <v>0</v>
       </c>
       <c r="AF46" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="AG46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AH46" s="54">
         <v>0</v>
@@ -28014,40 +28008,40 @@
         <v>0</v>
       </c>
       <c r="AJ46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AK46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AL46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AM46" s="54">
         <v>0</v>
       </c>
       <c r="AN46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AO46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AP46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AQ46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AR46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AS46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AT46" s="54">
         <v>0</v>
       </c>
       <c r="AU46" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AV46" s="5"/>
       <c r="AW46" s="5"/>
@@ -32954,13 +32948,13 @@
         <v>25</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D56" s="33" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E56" s="55" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F56" s="33">
         <v>90</v>
@@ -32978,7 +32972,7 @@
         <v>90</v>
       </c>
       <c r="K56" s="55" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L56" s="33">
         <v>90</v>
@@ -33005,7 +32999,7 @@
         <v>100</v>
       </c>
       <c r="T56" s="58" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="U56" s="17">
         <v>100</v>
@@ -33023,7 +33017,7 @@
         <v>100</v>
       </c>
       <c r="Z56" s="58" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="AA56" s="17">
         <v>100</v>
@@ -33050,7 +33044,7 @@
         <v>147</v>
       </c>
       <c r="AI56" s="59" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="AJ56" s="21">
         <v>147</v>
@@ -33068,7 +33062,7 @@
         <v>147</v>
       </c>
       <c r="AO56" s="59" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="AP56" s="21">
         <v>147</v>
@@ -33921,13 +33915,13 @@
         <v>26</v>
       </c>
       <c r="C57" s="57" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D57" s="57" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E57" s="56" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F57" s="33">
         <v>90</v>
@@ -33948,7 +33942,7 @@
         <v>90</v>
       </c>
       <c r="L57" s="56" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="M57" s="33">
         <v>90</v>
@@ -33972,7 +33966,7 @@
         <v>100</v>
       </c>
       <c r="T57" s="58" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="U57" s="17">
         <v>100</v>
@@ -33993,7 +33987,7 @@
         <v>100</v>
       </c>
       <c r="AA57" s="58" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="AB57" s="17">
         <v>100</v>
@@ -34017,7 +34011,7 @@
         <v>147</v>
       </c>
       <c r="AI57" s="59" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="AJ57" s="21">
         <v>147</v>
@@ -34038,7 +34032,7 @@
         <v>147</v>
       </c>
       <c r="AP57" s="59" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="AQ57" s="21">
         <v>147</v>
@@ -34888,13 +34882,13 @@
         <v>27</v>
       </c>
       <c r="C58" s="57" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D58" s="57" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E58" s="56" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F58" s="33">
         <v>170</v>
@@ -34918,7 +34912,7 @@
         <v>170</v>
       </c>
       <c r="M58" s="56" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="N58" s="33">
         <v>170</v>
@@ -34939,7 +34933,7 @@
         <v>180</v>
       </c>
       <c r="T58" s="58" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="U58" s="17">
         <v>180</v>
@@ -34963,7 +34957,7 @@
         <v>180</v>
       </c>
       <c r="AB58" s="58" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="AC58" s="17">
         <v>180</v>
@@ -34984,7 +34978,7 @@
         <v>375</v>
       </c>
       <c r="AI58" s="59" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="AJ58" s="21">
         <v>375</v>
@@ -35008,7 +35002,7 @@
         <v>375</v>
       </c>
       <c r="AQ58" s="59" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="AR58" s="21">
         <v>375</v>
@@ -35855,13 +35849,13 @@
         <v>28</v>
       </c>
       <c r="C59" s="57" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D59" s="57" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E59" s="56" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F59" s="33">
         <v>170</v>
@@ -35888,7 +35882,7 @@
         <v>170</v>
       </c>
       <c r="N59" s="56" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="O59" s="33">
         <v>170</v>
@@ -35906,7 +35900,7 @@
         <v>180</v>
       </c>
       <c r="T59" s="58" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="U59" s="17">
         <v>180</v>
@@ -35933,7 +35927,7 @@
         <v>180</v>
       </c>
       <c r="AC59" s="58" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="AD59" s="17">
         <v>180</v>
@@ -35951,7 +35945,7 @@
         <v>375</v>
       </c>
       <c r="AI59" s="59" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="AJ59" s="21">
         <v>375</v>
@@ -35978,7 +35972,7 @@
         <v>375</v>
       </c>
       <c r="AR59" s="59" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="AS59" s="21">
         <v>375</v>
@@ -36822,13 +36816,13 @@
         <v>29</v>
       </c>
       <c r="C60" s="57" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D60" s="57" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E60" s="56" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F60" s="33">
         <v>255</v>
@@ -36858,7 +36852,7 @@
         <v>255</v>
       </c>
       <c r="O60" s="56" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="P60" s="33">
         <v>255</v>
@@ -36873,7 +36867,7 @@
         <v>240</v>
       </c>
       <c r="T60" s="58" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="U60" s="17">
         <v>240</v>
@@ -36903,7 +36897,7 @@
         <v>240</v>
       </c>
       <c r="AD60" s="58" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="AE60" s="17">
         <v>240</v>
@@ -36918,7 +36912,7 @@
         <v>550</v>
       </c>
       <c r="AI60" s="59" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="AJ60" s="21">
         <v>550</v>
@@ -36948,7 +36942,7 @@
         <v>550</v>
       </c>
       <c r="AS60" s="59" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="AT60" s="21">
         <v>550</v>
@@ -37789,13 +37783,13 @@
         <v>29</v>
       </c>
       <c r="C61" s="57" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D61" s="57" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E61" s="56" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F61" s="33">
         <v>255</v>
@@ -37828,7 +37822,7 @@
         <v>255</v>
       </c>
       <c r="P61" s="56" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="Q61" s="33">
         <v>255</v>
@@ -37840,7 +37834,7 @@
         <v>240</v>
       </c>
       <c r="T61" s="58" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="U61" s="17">
         <v>240</v>
@@ -37873,7 +37867,7 @@
         <v>240</v>
       </c>
       <c r="AE61" s="58" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="AF61" s="17">
         <v>240</v>
@@ -37885,7 +37879,7 @@
         <v>550</v>
       </c>
       <c r="AI61" s="59" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="AJ61" s="21">
         <v>550</v>
@@ -37918,7 +37912,7 @@
         <v>550</v>
       </c>
       <c r="AT61" s="59" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="AU61" s="21">
         <v>550</v>
@@ -38753,13 +38747,13 @@
         <v>145</v>
       </c>
       <c r="C62" s="57" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D62" s="57" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E62" s="56" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F62" s="33">
         <v>255</v>
@@ -38795,7 +38789,7 @@
         <v>255</v>
       </c>
       <c r="Q62" s="56" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="R62" s="17">
         <v>0</v>
@@ -40752,7 +40746,7 @@
         <v>182</v>
       </c>
       <c r="E69" s="55" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F69" s="33" t="s">
         <v>182</v>
@@ -40770,7 +40764,7 @@
         <v>182</v>
       </c>
       <c r="K69" s="55" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="L69" s="33" t="s">
         <v>182</v>
@@ -40797,7 +40791,7 @@
         <v>182</v>
       </c>
       <c r="T69" s="48" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="U69" s="17" t="s">
         <v>182</v>
@@ -40815,7 +40809,7 @@
         <v>182</v>
       </c>
       <c r="Z69" s="48" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="AA69" s="17" t="s">
         <v>182</v>
@@ -40842,7 +40836,7 @@
         <v>188</v>
       </c>
       <c r="AI69" s="50" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="AJ69" s="21" t="s">
         <v>188</v>
@@ -40860,7 +40854,7 @@
         <v>188</v>
       </c>
       <c r="AO69" s="50" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="AP69" s="21" t="s">
         <v>188</v>
@@ -41719,7 +41713,7 @@
         <v>183</v>
       </c>
       <c r="E70" s="55" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F70" s="33" t="s">
         <v>183</v>
@@ -41743,7 +41737,7 @@
         <v>183</v>
       </c>
       <c r="M70" s="55" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="N70" s="33" t="s">
         <v>183</v>
@@ -41764,7 +41758,7 @@
         <v>183</v>
       </c>
       <c r="T70" s="48" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="U70" s="17" t="s">
         <v>183</v>
@@ -41788,7 +41782,7 @@
         <v>183</v>
       </c>
       <c r="AB70" s="48" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="AC70" s="17" t="s">
         <v>183</v>
@@ -41809,7 +41803,7 @@
         <v>189</v>
       </c>
       <c r="AI70" s="50" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="AJ70" s="21" t="s">
         <v>189</v>
@@ -41833,7 +41827,7 @@
         <v>189</v>
       </c>
       <c r="AQ70" s="50" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="AR70" s="21" t="s">
         <v>189</v>
@@ -42686,7 +42680,7 @@
         <v>184</v>
       </c>
       <c r="E71" s="55" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F71" s="33" t="s">
         <v>184</v>
@@ -42716,7 +42710,7 @@
         <v>184</v>
       </c>
       <c r="O71" s="55" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="P71" s="33" t="s">
         <v>184</v>
@@ -42731,7 +42725,7 @@
         <v>184</v>
       </c>
       <c r="T71" s="48" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="U71" s="17" t="s">
         <v>184</v>
@@ -42761,7 +42755,7 @@
         <v>184</v>
       </c>
       <c r="AD71" s="48" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="AE71" s="17" t="s">
         <v>184</v>
@@ -42776,7 +42770,7 @@
         <v>190</v>
       </c>
       <c r="AI71" s="50" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="AJ71" s="21" t="s">
         <v>190</v>
@@ -42806,7 +42800,7 @@
         <v>190</v>
       </c>
       <c r="AS71" s="50" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="AT71" s="21" t="s">
         <v>190</v>
@@ -43653,7 +43647,7 @@
         <v>185</v>
       </c>
       <c r="E72" s="55" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F72" s="33" t="s">
         <v>185</v>
@@ -43674,7 +43668,7 @@
         <v>185</v>
       </c>
       <c r="L72" s="55" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="M72" s="33" t="s">
         <v>185</v>
@@ -43698,7 +43692,7 @@
         <v>185</v>
       </c>
       <c r="T72" s="48" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="U72" s="17" t="s">
         <v>185</v>
@@ -43719,7 +43713,7 @@
         <v>185</v>
       </c>
       <c r="AA72" s="48" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="AB72" s="17" t="s">
         <v>185</v>
@@ -43743,7 +43737,7 @@
         <v>191</v>
       </c>
       <c r="AI72" s="50" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="AJ72" s="21" t="s">
         <v>191</v>
@@ -43764,7 +43758,7 @@
         <v>191</v>
       </c>
       <c r="AP72" s="50" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="AQ72" s="21" t="s">
         <v>191</v>
@@ -44620,7 +44614,7 @@
         <v>186</v>
       </c>
       <c r="E73" s="55" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F73" s="33" t="s">
         <v>186</v>
@@ -44647,7 +44641,7 @@
         <v>186</v>
       </c>
       <c r="N73" s="55" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="O73" s="33" t="s">
         <v>186</v>
@@ -44665,7 +44659,7 @@
         <v>186</v>
       </c>
       <c r="T73" s="48" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="U73" s="17" t="s">
         <v>186</v>
@@ -44692,7 +44686,7 @@
         <v>186</v>
       </c>
       <c r="AC73" s="48" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="AD73" s="17" t="s">
         <v>186</v>
@@ -44710,7 +44704,7 @@
         <v>192</v>
       </c>
       <c r="AI73" s="50" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="AJ73" s="21" t="s">
         <v>192</v>
@@ -44737,7 +44731,7 @@
         <v>192</v>
       </c>
       <c r="AR73" s="50" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="AS73" s="21" t="s">
         <v>192</v>
@@ -45587,7 +45581,7 @@
         <v>187</v>
       </c>
       <c r="E74" s="55" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F74" s="33" t="s">
         <v>187</v>
@@ -45620,7 +45614,7 @@
         <v>187</v>
       </c>
       <c r="P74" s="55" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="Q74" s="33" t="s">
         <v>187</v>
@@ -45632,7 +45626,7 @@
         <v>187</v>
       </c>
       <c r="T74" s="48" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="U74" s="17" t="s">
         <v>187</v>
@@ -45665,7 +45659,7 @@
         <v>187</v>
       </c>
       <c r="AE74" s="48" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="AF74" s="17" t="s">
         <v>187</v>
@@ -45677,7 +45671,7 @@
         <v>193</v>
       </c>
       <c r="AI74" s="50" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="AJ74" s="21" t="s">
         <v>193</v>
@@ -45710,7 +45704,7 @@
         <v>193</v>
       </c>
       <c r="AT74" s="50" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="AU74" s="21" t="s">
         <v>193</v>
@@ -46551,7 +46545,7 @@
         <v>187</v>
       </c>
       <c r="E75" s="55" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F75" s="33" t="s">
         <v>187</v>
@@ -46587,7 +46581,7 @@
         <v>187</v>
       </c>
       <c r="Q75" s="55" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="R75" s="17">
         <v>0</v>

</xml_diff>